<commit_message>
learn something new about pointer
</commit_message>
<xml_diff>
--- a/self extend practice/pointer practice/0、指针、地址小实验 .xlsx
+++ b/self extend practice/pointer practice/0、指针、地址小实验 .xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>main</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,50 @@
   </si>
   <si>
     <t>6487 619</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不同类型变量在内存中存放情况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int *pi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>char *pc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>257</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>512</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>256</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指针变量基类型作用</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -178,7 +222,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -191,6 +235,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -198,6 +254,105 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>115888</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="直接箭头连接符 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="7442200" y="2247900"/>
+          <a:ext cx="1155700" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="直接箭头连接符 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="7473950" y="2324100"/>
+          <a:ext cx="1143000" cy="615950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -485,18 +640,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:I28"/>
+  <dimension ref="C1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="8" max="8" width="10.26953125" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9">
+    <row r="1" spans="3:15">
+      <c r="E1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="K1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="4" spans="3:15">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -505,7 +675,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="3:9">
+    <row r="5" spans="3:15">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -516,7 +686,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="3:9">
+    <row r="6" spans="3:15">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="3" t="s">
@@ -529,7 +699,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="3:9">
+    <row r="7" spans="3:15">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="3" t="s">
@@ -542,7 +712,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="3:9">
+    <row r="8" spans="3:15">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -551,7 +721,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="3:9">
+    <row r="9" spans="3:15">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -560,7 +730,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="3:9">
+    <row r="10" spans="3:15">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
@@ -572,8 +742,12 @@
         <v>4</v>
       </c>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="3:9">
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="3:15">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -581,8 +755,9 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="3:9">
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="3:15">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
@@ -592,8 +767,9 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="3:9">
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="3:15">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -601,8 +777,12 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="3:9">
+      <c r="L13" s="9"/>
+      <c r="O13" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -610,8 +790,9 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="3:9">
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="3:15">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -621,8 +802,9 @@
         <v>8</v>
       </c>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="3:9">
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="3:15">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
@@ -632,8 +814,9 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="3:9">
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="3:18">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -641,8 +824,12 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="3:9">
+      <c r="L17" s="8"/>
+      <c r="O17" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -650,8 +837,9 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="3:9">
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="3:18">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -661,8 +849,16 @@
         <v>9</v>
       </c>
       <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="3:9">
+      <c r="L19" s="8"/>
+      <c r="N19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+    </row>
+    <row r="20" spans="3:18">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
@@ -672,8 +868,22 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="3:9">
+      <c r="L20" s="8"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="R20" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -681,8 +891,16 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="3:9">
+      <c r="L21" s="8"/>
+      <c r="N21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+    </row>
+    <row r="22" spans="3:18">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -690,8 +908,22 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="3:9">
+      <c r="L22" s="8"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R22" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="3:18">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -701,8 +933,15 @@
         <v>14</v>
       </c>
       <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="3:9">
+      <c r="N23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+    </row>
+    <row r="24" spans="3:18">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
@@ -714,8 +953,21 @@
         <v>15</v>
       </c>
       <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="3:9">
+      <c r="N24" s="10"/>
+      <c r="O24" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q24" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="R24" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -723,8 +975,13 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="3:9">
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+    </row>
+    <row r="26" spans="3:18">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -734,8 +991,13 @@
         <v>5</v>
       </c>
       <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="3:9">
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+    </row>
+    <row r="27" spans="3:18">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -743,14 +1005,36 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="3:9">
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+    </row>
+    <row r="28" spans="3:18">
       <c r="F28" s="1"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+    </row>
+    <row r="29" spans="3:18">
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="K1:N1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>